<commit_message>
Arquivos corrigidos para a ultima avaliação
</commit_message>
<xml_diff>
--- a/23- Matrizes de Rastreabilidade (Características X SSS Incompleto).xlsx
+++ b/23- Matrizes de Rastreabilidade (Características X SSS Incompleto).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alisson\Desktop\Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\alisson jitador 2.o\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C3111A-E836-436E-80F1-8AD7A31B9C5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259AC23A-C51F-41AD-9521-2AB5266769B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D60DB500-E946-480D-9D30-5E3BDB6AD24C}"/>
+    <workbookView xWindow="2505" yWindow="2505" windowWidth="15300" windowHeight="7875" tabRatio="433" xr2:uid="{D60DB500-E946-480D-9D30-5E3BDB6AD24C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t>SSS-002</t>
   </si>
@@ -239,13 +239,22 @@
   <si>
     <t>Matrizes de Rastreabilidade (Características x SSS: incompleto)
  Matrizes de Rastreabilidade (Características x SSS: incompleto)</t>
+  </si>
+  <si>
+    <t>SSS-018</t>
+  </si>
+  <si>
+    <t>SSS-019</t>
+  </si>
+  <si>
+    <t>SSS-020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,6 +280,12 @@
       <b/>
       <sz val="15"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -655,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93112886-E03E-4619-8ECC-E03B753FE0DA}">
-  <dimension ref="A1:R58"/>
+  <dimension ref="A1:U58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="M40" workbookViewId="0">
+      <selection activeCell="V44" sqref="V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +681,7 @@
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="19.5" x14ac:dyDescent="0.3">
       <c r="B1" s="7" t="s">
         <v>70</v>
       </c>
@@ -687,7 +702,7 @@
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
     </row>
-    <row r="5" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>69</v>
       </c>
@@ -739,8 +754,17 @@
       <c r="R5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>16</v>
       </c>
@@ -760,8 +784,11 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -782,8 +809,11 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -804,8 +834,11 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-    </row>
-    <row r="9" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
@@ -826,8 +859,11 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-    </row>
-    <row r="10" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
@@ -848,8 +884,11 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -870,8 +909,11 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-    </row>
-    <row r="12" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -892,8 +934,11 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
@@ -916,8 +961,11 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-    </row>
-    <row r="14" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
@@ -938,8 +986,11 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -960,8 +1011,11 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -982,8 +1036,11 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1004,8 +1061,11 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>29</v>
       </c>
@@ -1026,8 +1086,11 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-    </row>
-    <row r="19" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>30</v>
       </c>
@@ -1048,8 +1111,11 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-    </row>
-    <row r="20" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
@@ -1070,8 +1136,11 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-    </row>
-    <row r="21" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
@@ -1092,8 +1161,11 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-    </row>
-    <row r="22" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>33</v>
       </c>
@@ -1114,8 +1186,11 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
-    </row>
-    <row r="23" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1138,8 +1213,11 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-    </row>
-    <row r="24" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1160,8 +1238,11 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-    </row>
-    <row r="25" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
@@ -1184,8 +1265,11 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
-    </row>
-    <row r="26" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>37</v>
       </c>
@@ -1206,8 +1290,11 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-    </row>
-    <row r="27" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
@@ -1228,8 +1315,11 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-    </row>
-    <row r="28" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>39</v>
       </c>
@@ -1250,8 +1340,11 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
-    </row>
-    <row r="29" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>40</v>
       </c>
@@ -1272,8 +1365,11 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
-    </row>
-    <row r="30" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>41</v>
       </c>
@@ -1294,8 +1390,11 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-    </row>
-    <row r="31" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>42</v>
       </c>
@@ -1316,8 +1415,11 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-    </row>
-    <row r="32" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>43</v>
       </c>
@@ -1338,8 +1440,11 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-    </row>
-    <row r="33" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>44</v>
       </c>
@@ -1360,8 +1465,11 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
-    </row>
-    <row r="34" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>45</v>
       </c>
@@ -1382,8 +1490,11 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
-    </row>
-    <row r="35" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="2"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>46</v>
       </c>
@@ -1404,8 +1515,11 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
-    </row>
-    <row r="36" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>47</v>
       </c>
@@ -1426,8 +1540,11 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
-    </row>
-    <row r="37" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="2"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>48</v>
       </c>
@@ -1450,8 +1567,11 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
-    </row>
-    <row r="38" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S37" s="2"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="2"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>49</v>
       </c>
@@ -1472,8 +1592,11 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
-    </row>
-    <row r="39" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>50</v>
       </c>
@@ -1498,8 +1621,11 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
-    </row>
-    <row r="40" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>51</v>
       </c>
@@ -1520,8 +1646,11 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
-    </row>
-    <row r="41" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>52</v>
       </c>
@@ -1542,8 +1671,11 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
-    </row>
-    <row r="42" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>53</v>
       </c>
@@ -1566,8 +1698,11 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
-    </row>
-    <row r="43" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>54</v>
       </c>
@@ -1594,8 +1729,13 @@
       </c>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
-    </row>
-    <row r="44" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>55</v>
       </c>
@@ -1618,8 +1758,11 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
-    </row>
-    <row r="45" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>56</v>
       </c>
@@ -1642,8 +1785,11 @@
       <c r="R45" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>57</v>
       </c>
@@ -1664,8 +1810,15 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
-    </row>
-    <row r="47" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S46" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="T46" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U46" s="2"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>58</v>
       </c>
@@ -1686,8 +1839,11 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
-    </row>
-    <row r="48" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S47" s="2"/>
+      <c r="T47" s="2"/>
+      <c r="U47" s="2"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>59</v>
       </c>
@@ -1710,8 +1866,11 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
-    </row>
-    <row r="49" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S48" s="2"/>
+      <c r="T48" s="2"/>
+      <c r="U48" s="2"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>60</v>
       </c>
@@ -1738,8 +1897,11 @@
         <v>24</v>
       </c>
       <c r="R49" s="2"/>
-    </row>
-    <row r="50" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S49" s="2"/>
+      <c r="T49" s="2"/>
+      <c r="U49" s="2"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>61</v>
       </c>
@@ -1760,8 +1922,11 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
-    </row>
-    <row r="51" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S50" s="2"/>
+      <c r="T50" s="2"/>
+      <c r="U50" s="2"/>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>62</v>
       </c>
@@ -1784,8 +1949,11 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
-    </row>
-    <row r="52" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S51" s="2"/>
+      <c r="T51" s="2"/>
+      <c r="U51" s="2"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>63</v>
       </c>
@@ -1806,8 +1974,11 @@
       <c r="P52" s="2"/>
       <c r="Q52" s="2"/>
       <c r="R52" s="2"/>
-    </row>
-    <row r="53" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S52" s="2"/>
+      <c r="T52" s="2"/>
+      <c r="U52" s="2"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>64</v>
       </c>
@@ -1830,8 +2001,11 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2"/>
-    </row>
-    <row r="54" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S53" s="2"/>
+      <c r="T53" s="2"/>
+      <c r="U53" s="2"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>65</v>
       </c>
@@ -1852,8 +2026,11 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2"/>
-    </row>
-    <row r="55" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S54" s="2"/>
+      <c r="T54" s="2"/>
+      <c r="U54" s="2"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>66</v>
       </c>
@@ -1874,8 +2051,11 @@
       <c r="P55" s="2"/>
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
-    </row>
-    <row r="56" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S55" s="2"/>
+      <c r="T55" s="2"/>
+      <c r="U55" s="2"/>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>67</v>
       </c>
@@ -1896,8 +2076,11 @@
       <c r="P56" s="2"/>
       <c r="Q56" s="2"/>
       <c r="R56" s="2"/>
-    </row>
-    <row r="57" spans="1:18" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="S56" s="2"/>
+      <c r="T56" s="2"/>
+      <c r="U56" s="2"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>68</v>
       </c>
@@ -1922,8 +2105,11 @@
       <c r="P57" s="4"/>
       <c r="Q57" s="4"/>
       <c r="R57" s="4"/>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S57" s="4"/>
+      <c r="T57" s="4"/>
+      <c r="U57" s="4"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B58">
         <v>1</v>
       </c>
@@ -1974,12 +2160,22 @@
       </c>
       <c r="R58">
         <v>17</v>
+      </c>
+      <c r="S58">
+        <v>18</v>
+      </c>
+      <c r="T58">
+        <v>19</v>
+      </c>
+      <c r="U58">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:R1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>